<commit_message>
Revising Mart 1 for specific tests and weekly report.
</commit_message>
<xml_diff>
--- a/Misc/DV Joiner Table.xlsx
+++ b/Misc/DV Joiner Table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amurphy/Documents/GitHub/TBI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amurphy/Documents/GitHub/Bureau_Analysis/Misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2737B6F5-04B4-934C-80A8-148038B6A086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{336B72DE-A419-F24E-A8A0-E4926A7AE8EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="21960" windowHeight="18820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="108">
   <si>
     <t>ORI</t>
   </si>
@@ -315,9 +315,6 @@
   </si>
   <si>
     <t>Primary Location</t>
-  </si>
-  <si>
-    <t>Secondary Location</t>
   </si>
   <si>
     <t>Mart 2 Requested:</t>
@@ -2716,7 +2713,7 @@
   <dimension ref="A2:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2786,7 +2783,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D7" t="s">
         <v>86</v>
@@ -2797,7 +2794,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D8" t="s">
         <v>87</v>
@@ -2830,18 +2827,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>97</v>
-      </c>
-      <c r="D11" t="s">
-        <v>75</v>
-      </c>
-      <c r="E11" s="24" t="s">
-        <v>94</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="E11" s="24"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -2851,7 +2843,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -2859,16 +2851,16 @@
         <v>24</v>
       </c>
       <c r="B16" t="s">
+        <v>104</v>
+      </c>
+      <c r="C16" t="s">
         <v>105</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>106</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>107</v>
-      </c>
-      <c r="E16" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
@@ -2883,7 +2875,7 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
@@ -2893,22 +2885,22 @@
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>